<commit_message>
add Marks page + download template
</commit_message>
<xml_diff>
--- a/public/assets/templates/student-list-template.xlsx
+++ b/public/assets/templates/student-list-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni_Learning\PROJECT\HKI 21-22\gradebook-fe\public\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be785d2873c8d679/Máy tính/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5117E9B5-CC30-4C1B-9E98-632A8D210BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{520E433D-A8FB-48BE-8371-DDBA3469701D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26967A0-CD65-42A4-ADD1-1AA99EB454F8}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" xr2:uid="{9ADA3558-F44A-4AE6-99A2-143E50887A4F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Student ID</t>
   </si>
   <si>
-    <t>Fullname</t>
+    <t>Point</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
show & edit student grade
</commit_message>
<xml_diff>
--- a/public/assets/templates/student-list-template.xlsx
+++ b/public/assets/templates/student-list-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be785d2873c8d679/Máy tính/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni_Learning\PROJECT\HKI 21-22\gradebook-fe\public\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{520E433D-A8FB-48BE-8371-DDBA3469701D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26967A0-CD65-42A4-ADD1-1AA99EB454F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5117E9B5-CC30-4C1B-9E98-632A8D210BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" xr2:uid="{9ADA3558-F44A-4AE6-99A2-143E50887A4F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>Student ID</t>
   </si>
   <si>
-    <t>Point</t>
+    <t>Fullname</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>